<commit_message>
Tab 3 - Phase 1
</commit_message>
<xml_diff>
--- a/Assets/Files/Groundwater/HydrographData_Template.xlsx
+++ b/Assets/Files/Groundwater/HydrographData_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\pooya\w\KHRW-DASHBOARD\Assets\Files\Groundwater\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\shirazipooya\w\KHRW-DASHBOARD\Assets\Files\Groundwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4DE051-B70B-4C10-A3EE-700170D62F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CF7C42-376C-40AE-9F98-6106BF7F605A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{1C20E691-FEDC-4DDF-9376-FE14AAC707BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1C20E691-FEDC-4DDF-9376-FE14AAC707BD}"/>
   </bookViews>
   <sheets>
     <sheet name="GeoInfo" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>XUTM</t>
   </si>
@@ -34,24 +34,15 @@
     <t>YUTM</t>
   </si>
   <si>
-    <t>MAHDOUDE_CODE</t>
-  </si>
-  <si>
     <t>MAHDOUDE_NAME</t>
   </si>
   <si>
     <t>LOCATION_NAME</t>
   </si>
   <si>
-    <t>INFO</t>
-  </si>
-  <si>
     <t>THISSEN_LOCATION</t>
   </si>
   <si>
-    <t>NO_MEASURE_CODE</t>
-  </si>
-  <si>
     <t>ZONEUTM</t>
   </si>
   <si>
@@ -61,12 +52,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>MIN_YEAR</t>
-  </si>
-  <si>
-    <t>MAX_YEAR</t>
-  </si>
-  <si>
     <t>AQUIFER_NAME</t>
   </si>
   <si>
@@ -76,15 +61,6 @@
     <t>LEVEL_SRTM</t>
   </si>
   <si>
-    <t>DATE_GREGORIAN_RAW</t>
-  </si>
-  <si>
-    <t>DATE_PERSIAN_RAW</t>
-  </si>
-  <si>
-    <t>WATER_TABLE_RAW</t>
-  </si>
-  <si>
     <t>THISSEN_AQUIFER</t>
   </si>
   <si>
@@ -94,10 +70,40 @@
     <t>سرخس</t>
   </si>
   <si>
-    <t>DATA_STATE</t>
-  </si>
-  <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>YEAR_PERSIAN</t>
+  </si>
+  <si>
+    <t>MONTH_PERSIAN</t>
+  </si>
+  <si>
+    <t>DAY_PERSIAN</t>
+  </si>
+  <si>
+    <t>DATE_PERSIAN</t>
+  </si>
+  <si>
+    <t>YEAR_GREGORIAN</t>
+  </si>
+  <si>
+    <t>MONTH_GREGORIAN</t>
+  </si>
+  <si>
+    <t>DAY_GREGORIAN</t>
+  </si>
+  <si>
+    <t>DATE_GREGORIAN</t>
+  </si>
+  <si>
+    <t>WATER_TABLE</t>
+  </si>
+  <si>
+    <t>STORAGE_COEFFICIENT_AQUIFER</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -107,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,21 +135,13 @@
       <charset val="178"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="B Mitra"/>
       <charset val="178"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,31 +168,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -202,25 +182,15 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -228,15 +198,125 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="32">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Mitra"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Mitra"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Mitra"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Mitra"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Mitra"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -483,84 +563,6 @@
         <charset val="178"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -800,25 +802,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -834,49 +817,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{605F0EEF-2587-4449-BB76-744A91B8683C}" name="Table13" displayName="Table13" ref="A1:N2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:N2" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{9D5DEE88-C328-4677-8D3D-1CC93EE54576}" name="ID" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{C120709A-470D-4432-9660-E4359E62912B}" name="MAHDOUDE_NAME" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{21673562-BA39-487B-9F8C-58653E2AABE9}" name="MAHDOUDE_CODE" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{A034B5D8-C49D-4436-AC08-6ABDB53DCAF4}" name="AQUIFER_NAME" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{2AD3FCA4-ABB3-4D1B-8B91-CCD8C2F655A0}" name="LOCATION_NAME" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{91E11DF4-7191-49CE-A81D-71BE1B094777}" name="XUTM" dataDxfId="22" dataCellStyle="Comma"/>
-    <tableColumn id="10" xr3:uid="{7479EB79-7A7C-4364-B299-5CA06A862179}" name="YUTM" dataDxfId="21" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{0650D9A9-E841-4607-9AFC-02905FF45290}" name="ZONEUTM" dataDxfId="20" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{8F567313-DCB8-4136-95D5-5DEC11AC28A1}" name="X" dataDxfId="19" dataCellStyle="Comma"/>
-    <tableColumn id="13" xr3:uid="{BC8FEB10-A445-480C-8334-D126AE35456C}" name="Y" dataDxfId="18" dataCellStyle="Comma"/>
-    <tableColumn id="14" xr3:uid="{67E1939A-40CF-47CC-B14E-47277853E3FF}" name="MIN_YEAR" dataDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="15" xr3:uid="{7F99A8C9-1642-45BA-8D1A-591F13CD6C0E}" name="MAX_YEAR" dataDxfId="16" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{1321A389-2C01-4126-B7A1-04C2D21B2125}" name="LEVEL_MSL" dataDxfId="15" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{4204419C-7DF3-4285-A2B0-1BF1EB459E98}" name="LEVEL_SRTM" dataDxfId="14" dataCellStyle="Comma"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{605F0EEF-2587-4449-BB76-744A91B8683C}" name="Table13" displayName="Table13" ref="A1:K2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="31">
+  <autoFilter ref="A1:K2" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{9D5DEE88-C328-4677-8D3D-1CC93EE54576}" name="ID" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{C120709A-470D-4432-9660-E4359E62912B}" name="MAHDOUDE_NAME" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{21673562-BA39-487B-9F8C-58653E2AABE9}" name="AQUIFER_NAME" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{A034B5D8-C49D-4436-AC08-6ABDB53DCAF4}" name="LOCATION_NAME" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{2AD3FCA4-ABB3-4D1B-8B91-CCD8C2F655A0}" name="XUTM" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{91E11DF4-7191-49CE-A81D-71BE1B094777}" name="YUTM" dataDxfId="25" dataCellStyle="Comma"/>
+    <tableColumn id="10" xr3:uid="{7479EB79-7A7C-4364-B299-5CA06A862179}" name="ZONEUTM" dataDxfId="24" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{0650D9A9-E841-4607-9AFC-02905FF45290}" name="X" dataDxfId="23" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{8F567313-DCB8-4136-95D5-5DEC11AC28A1}" name="Y" dataDxfId="22" dataCellStyle="Comma"/>
+    <tableColumn id="13" xr3:uid="{BC8FEB10-A445-480C-8334-D126AE35456C}" name="LEVEL_MSL" dataDxfId="21" dataCellStyle="Comma"/>
+    <tableColumn id="14" xr3:uid="{67E1939A-40CF-47CC-B14E-47277853E3FF}" name="LEVEL_SRTM" dataDxfId="20" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}" name="Table1" displayName="Table1" ref="A1:L2" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L2" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}" name="Table1" displayName="Table1" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="19">
+  <autoFilter ref="A1:Q2" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L2">
     <sortCondition ref="B2"/>
     <sortCondition ref="C2"/>
     <sortCondition ref="E2"/>
   </sortState>
-  <tableColumns count="12">
-    <tableColumn id="6" xr3:uid="{D5CEC73D-60D1-4068-ACEC-156E1DCE1D3B}" name="MAHDOUDE_NAME" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{B5416EAC-6728-48AC-9FCF-891BE4987A0D}" name="AQUIFER_NAME" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{7358129A-5416-4405-8D01-C5FA18520307}" name="LOCATION_NAME" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{B4264AD6-D9ED-427B-9D46-D0AECFE7FF43}" name="DATA_STATE" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{14A3C0B2-EE2E-4B75-A733-DEB76AC3F7B1}" name="DATE_PERSIAN_RAW" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{A9B88317-08A6-439A-BE52-CAF0D92F768F}" name="DATE_GREGORIAN_RAW" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{53B15055-68C7-44E4-B89C-0C08F72CB6C7}" name="WATER_TABLE_RAW" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{391B65EA-408D-42B5-9D89-6F4F102FC98A}" name="NO_MEASURE_CODE" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{314EBD28-38AE-4E79-A21E-E31B82BBC375}" name="INFO" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{606896FC-817F-49C6-8BE2-6F871089F4EB}" name="STORAGE_COEFFICIENT_LOCATION" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{D0E411EF-08E3-4C7C-B147-1FA4CFA513AB}" name="THISSEN_LOCATION" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="15" xr3:uid="{3D10739D-F1D1-47F1-9B2B-CA84D92739C7}" name="THISSEN_AQUIFER" dataDxfId="0" dataCellStyle="Comma"/>
+  <tableColumns count="17">
+    <tableColumn id="6" xr3:uid="{D5CEC73D-60D1-4068-ACEC-156E1DCE1D3B}" name="MAHDOUDE_NAME" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{B5416EAC-6728-48AC-9FCF-891BE4987A0D}" name="AQUIFER_NAME" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{7358129A-5416-4405-8D01-C5FA18520307}" name="LOCATION_NAME" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{B4264AD6-D9ED-427B-9D46-D0AECFE7FF43}" name="YEAR_PERSIAN" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{14A3C0B2-EE2E-4B75-A733-DEB76AC3F7B1}" name="MONTH_PERSIAN" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{A9B88317-08A6-439A-BE52-CAF0D92F768F}" name="DAY_PERSIAN" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{53B15055-68C7-44E4-B89C-0C08F72CB6C7}" name="DATE_PERSIAN" dataDxfId="12" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{391B65EA-408D-42B5-9D89-6F4F102FC98A}" name="YEAR_GREGORIAN" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{314EBD28-38AE-4E79-A21E-E31B82BBC375}" name="MONTH_GREGORIAN" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{606896FC-817F-49C6-8BE2-6F871089F4EB}" name="DAY_GREGORIAN" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{D0E411EF-08E3-4C7C-B147-1FA4CFA513AB}" name="DATE_GREGORIAN" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="15" xr3:uid="{3D10739D-F1D1-47F1-9B2B-CA84D92739C7}" name="WATER_TABLE" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{79EF02DB-BA65-4263-9774-94B48720776B}" name="STORAGE_COEFFICIENT_LOCATION" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{13659474-902F-43D8-A178-4DF2AA611C8D}" name="STORAGE_COEFFICIENT_AQUIFER" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{60031051-C2EC-43B2-BC33-8524170B3A8F}" name="THISSEN_LOCATION" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{63DC3AD9-7AD7-4DE9-868F-C641776FC666}" name="THISSEN_AQUIFER" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{1AF4D720-014A-4007-8BCB-C8F2BDFE2825}" name="DESCRIPTION" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1179,81 +1164,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FDD836-E936-4393-A59B-21BB37D1D90D}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="17.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="12" customWidth="1"/>
-    <col min="7" max="8" width="10.6640625" style="9" customWidth="1"/>
-    <col min="9" max="10" width="7.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" style="10" customWidth="1"/>
-    <col min="12" max="13" width="14.33203125" style="11" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:11" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="3"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1263,80 +1240,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0079320B-CF91-4CBB-8106-32433F29B95C}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
-    <col min="7" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="27.88671875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="17.109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:17" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="11"/>
+      <c r="G2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Start Tab Wells Data Visualizitation
</commit_message>
<xml_diff>
--- a/Assets/Files/Groundwater/HydrographData_Template.xlsx
+++ b/Assets/Files/Groundwater/HydrographData_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\shirazipooya\w\KHRW-DASHBOARD\Assets\Files\Groundwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CF7C42-376C-40AE-9F98-6106BF7F605A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6064409-5EA5-4BE9-B337-03E9F8841D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1C20E691-FEDC-4DDF-9376-FE14AAC707BD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C20E691-FEDC-4DDF-9376-FE14AAC707BD}"/>
   </bookViews>
   <sheets>
     <sheet name="GeoInfo" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>XUTM</t>
   </si>
@@ -40,9 +40,6 @@
     <t>LOCATION_NAME</t>
   </si>
   <si>
-    <t>THISSEN_LOCATION</t>
-  </si>
-  <si>
     <t>ZONEUTM</t>
   </si>
   <si>
@@ -61,12 +58,6 @@
     <t>LEVEL_SRTM</t>
   </si>
   <si>
-    <t>THISSEN_AQUIFER</t>
-  </si>
-  <si>
-    <t>STORAGE_COEFFICIENT_LOCATION</t>
-  </si>
-  <si>
     <t>سرخس</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
   </si>
   <si>
     <t>WATER_TABLE</t>
-  </si>
-  <si>
-    <t>STORAGE_COEFFICIENT_AQUIFER</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -215,107 +203,25 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="B Mitra"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="B Mitra"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -563,6 +469,9 @@
         <charset val="178"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -802,6 +711,9 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -817,51 +729,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{605F0EEF-2587-4449-BB76-744A91B8683C}" name="Table13" displayName="Table13" ref="A1:K2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{605F0EEF-2587-4449-BB76-744A91B8683C}" name="Table13" displayName="Table13" ref="A1:K2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:K2" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{9D5DEE88-C328-4677-8D3D-1CC93EE54576}" name="ID" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{C120709A-470D-4432-9660-E4359E62912B}" name="MAHDOUDE_NAME" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{21673562-BA39-487B-9F8C-58653E2AABE9}" name="AQUIFER_NAME" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{A034B5D8-C49D-4436-AC08-6ABDB53DCAF4}" name="LOCATION_NAME" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{2AD3FCA4-ABB3-4D1B-8B91-CCD8C2F655A0}" name="XUTM" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{91E11DF4-7191-49CE-A81D-71BE1B094777}" name="YUTM" dataDxfId="25" dataCellStyle="Comma"/>
-    <tableColumn id="10" xr3:uid="{7479EB79-7A7C-4364-B299-5CA06A862179}" name="ZONEUTM" dataDxfId="24" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{0650D9A9-E841-4607-9AFC-02905FF45290}" name="X" dataDxfId="23" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{8F567313-DCB8-4136-95D5-5DEC11AC28A1}" name="Y" dataDxfId="22" dataCellStyle="Comma"/>
-    <tableColumn id="13" xr3:uid="{BC8FEB10-A445-480C-8334-D126AE35456C}" name="LEVEL_MSL" dataDxfId="21" dataCellStyle="Comma"/>
-    <tableColumn id="14" xr3:uid="{67E1939A-40CF-47CC-B14E-47277853E3FF}" name="LEVEL_SRTM" dataDxfId="20" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{9D5DEE88-C328-4677-8D3D-1CC93EE54576}" name="ID" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{C120709A-470D-4432-9660-E4359E62912B}" name="MAHDOUDE_NAME" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{21673562-BA39-487B-9F8C-58653E2AABE9}" name="AQUIFER_NAME" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{A034B5D8-C49D-4436-AC08-6ABDB53DCAF4}" name="LOCATION_NAME" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{2AD3FCA4-ABB3-4D1B-8B91-CCD8C2F655A0}" name="XUTM" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{91E11DF4-7191-49CE-A81D-71BE1B094777}" name="YUTM" dataDxfId="20" dataCellStyle="Comma"/>
+    <tableColumn id="10" xr3:uid="{7479EB79-7A7C-4364-B299-5CA06A862179}" name="ZONEUTM" dataDxfId="19" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{0650D9A9-E841-4607-9AFC-02905FF45290}" name="X" dataDxfId="18" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{8F567313-DCB8-4136-95D5-5DEC11AC28A1}" name="Y" dataDxfId="17" dataCellStyle="Comma"/>
+    <tableColumn id="13" xr3:uid="{BC8FEB10-A445-480C-8334-D126AE35456C}" name="LEVEL_MSL" dataDxfId="16" dataCellStyle="Comma"/>
+    <tableColumn id="14" xr3:uid="{67E1939A-40CF-47CC-B14E-47277853E3FF}" name="LEVEL_SRTM" dataDxfId="15" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}" name="Table1" displayName="Table1" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="19">
-  <autoFilter ref="A1:Q2" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}" name="Table1" displayName="Table1" ref="A1:M2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:M2" xr:uid="{47D92E55-0C8F-40DE-A232-4C461AAFF479}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L2">
     <sortCondition ref="B2"/>
     <sortCondition ref="C2"/>
     <sortCondition ref="E2"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="6" xr3:uid="{D5CEC73D-60D1-4068-ACEC-156E1DCE1D3B}" name="MAHDOUDE_NAME" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{B5416EAC-6728-48AC-9FCF-891BE4987A0D}" name="AQUIFER_NAME" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{7358129A-5416-4405-8D01-C5FA18520307}" name="LOCATION_NAME" dataDxfId="16"/>
-    <tableColumn id="1" xr3:uid="{B4264AD6-D9ED-427B-9D46-D0AECFE7FF43}" name="YEAR_PERSIAN" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{14A3C0B2-EE2E-4B75-A733-DEB76AC3F7B1}" name="MONTH_PERSIAN" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{A9B88317-08A6-439A-BE52-CAF0D92F768F}" name="DAY_PERSIAN" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{53B15055-68C7-44E4-B89C-0C08F72CB6C7}" name="DATE_PERSIAN" dataDxfId="12" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{391B65EA-408D-42B5-9D89-6F4F102FC98A}" name="YEAR_GREGORIAN" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{314EBD28-38AE-4E79-A21E-E31B82BBC375}" name="MONTH_GREGORIAN" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{606896FC-817F-49C6-8BE2-6F871089F4EB}" name="DAY_GREGORIAN" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{D0E411EF-08E3-4C7C-B147-1FA4CFA513AB}" name="DATE_GREGORIAN" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="15" xr3:uid="{3D10739D-F1D1-47F1-9B2B-CA84D92739C7}" name="WATER_TABLE" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{79EF02DB-BA65-4263-9774-94B48720776B}" name="STORAGE_COEFFICIENT_LOCATION" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{13659474-902F-43D8-A178-4DF2AA611C8D}" name="STORAGE_COEFFICIENT_AQUIFER" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{60031051-C2EC-43B2-BC33-8524170B3A8F}" name="THISSEN_LOCATION" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{63DC3AD9-7AD7-4DE9-868F-C641776FC666}" name="THISSEN_AQUIFER" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{1AF4D720-014A-4007-8BCB-C8F2BDFE2825}" name="DESCRIPTION" dataDxfId="1"/>
+  <tableColumns count="13">
+    <tableColumn id="6" xr3:uid="{D5CEC73D-60D1-4068-ACEC-156E1DCE1D3B}" name="MAHDOUDE_NAME" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{B5416EAC-6728-48AC-9FCF-891BE4987A0D}" name="AQUIFER_NAME" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{7358129A-5416-4405-8D01-C5FA18520307}" name="LOCATION_NAME" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{B4264AD6-D9ED-427B-9D46-D0AECFE7FF43}" name="YEAR_PERSIAN" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{14A3C0B2-EE2E-4B75-A733-DEB76AC3F7B1}" name="MONTH_PERSIAN" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{A9B88317-08A6-439A-BE52-CAF0D92F768F}" name="DAY_PERSIAN" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{53B15055-68C7-44E4-B89C-0C08F72CB6C7}" name="DATE_PERSIAN" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{391B65EA-408D-42B5-9D89-6F4F102FC98A}" name="YEAR_GREGORIAN" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{314EBD28-38AE-4E79-A21E-E31B82BBC375}" name="MONTH_GREGORIAN" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{606896FC-817F-49C6-8BE2-6F871089F4EB}" name="DAY_GREGORIAN" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{D0E411EF-08E3-4C7C-B147-1FA4CFA513AB}" name="DATE_GREGORIAN" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="15" xr3:uid="{3D10739D-F1D1-47F1-9B2B-CA84D92739C7}" name="WATER_TABLE" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="17" xr3:uid="{1AF4D720-014A-4007-8BCB-C8F2BDFE2825}" name="DESCRIPTION" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1188,13 +1096,13 @@
   <sheetData>
     <row r="1" spans="1:11" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3</v>
@@ -1206,19 +1114,19 @@
         <v>1</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1240,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0079320B-CF91-4CBB-8106-32433F29B95C}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1260,70 +1168,54 @@
     <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="1"/>
+    <col min="13" max="13" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="11"/>

</xml_diff>